<commit_message>
ants felt work Original hash: a6375e06c972f601d5b28b9472de051f0448aacb
</commit_message>
<xml_diff>
--- a/AudioAnalysis/FELT/FELT/ExcelResultsComputationTemplate.xlsx
+++ b/AudioAnalysis/FELT/FELT/ExcelResultsComputationTemplate.xlsx
@@ -2,21 +2,24 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="18195" windowHeight="12210"/>
+    <workbookView xWindow="480" yWindow="360" windowWidth="18195" windowHeight="12090"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
     <sheet name="SummaryChart" sheetId="6" r:id="rId2"/>
     <sheet name="Summary Results" sheetId="3" r:id="rId3"/>
-    <sheet name="Full Results" sheetId="2" r:id="rId4"/>
-    <sheet name="Full Results Distances" sheetId="5" r:id="rId5"/>
+    <sheet name="RocChart" sheetId="8" r:id="rId4"/>
+    <sheet name="ROCData" sheetId="7" r:id="rId5"/>
+    <sheet name="Full Results" sheetId="2" r:id="rId6"/>
+    <sheet name="Full Results Distances" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="AlgorithmDetails">Log!$C$9</definedName>
     <definedName name="AlgorithmName">Log!$C$8</definedName>
     <definedName name="AlgorithmType">Log!$C$7</definedName>
+    <definedName name="ConfusionReport">Log!$A$37</definedName>
     <definedName name="FeatureDataTypes">Log!$C$11</definedName>
     <definedName name="FeatureNames">Log!$C$12</definedName>
     <definedName name="frClasses">'Full Results'!$A$2</definedName>
@@ -27,8 +30,12 @@
     <definedName name="frNumbers">'Full Results'!$C$1</definedName>
     <definedName name="frPlaces">'Full Results'!$B$2</definedName>
     <definedName name="MemUsage">Log!$F$5</definedName>
+    <definedName name="Negatives">Log!$H$17</definedName>
     <definedName name="PercentileSummary">Log!$F$22</definedName>
     <definedName name="PlacementSummary">Log!$B$22</definedName>
+    <definedName name="Positives">Log!$H$16</definedName>
+    <definedName name="RocCurveData">ROCData!$H$2</definedName>
+    <definedName name="RocSummary">ROCData!$A$2</definedName>
     <definedName name="RunDate">Log!$B$2</definedName>
     <definedName name="srPlaces">'Summary Results'!$A$2</definedName>
     <definedName name="TagSummary">Log!$B$16</definedName>
@@ -36,9 +43,12 @@
     <definedName name="TestEndInstanceCount">Log!$C$17</definedName>
     <definedName name="TimeTaken">Log!$F$4</definedName>
     <definedName name="TrBytes">Log!$B$4</definedName>
+    <definedName name="TrueNegatives">Log!$H$17</definedName>
+    <definedName name="TruePositives">Log!$H$16</definedName>
     <definedName name="Version">Log!$B$3</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -77,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="70">
   <si>
     <t>FELT TOOL</t>
   </si>
@@ -127,9 +137,6 @@
     <t>Count</t>
   </si>
   <si>
-    <t>%</t>
-  </si>
-  <si>
     <t>FELT Version</t>
   </si>
   <si>
@@ -182,6 +189,114 @@
   </si>
   <si>
     <t>Configuration</t>
+  </si>
+  <si>
+    <t>True Positives</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>Test (total)</t>
+  </si>
+  <si>
+    <t>Correct total?</t>
+  </si>
+  <si>
+    <t>Postives</t>
+  </si>
+  <si>
+    <t>Negatives</t>
+  </si>
+  <si>
+    <t>Roc Area</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Total Positives</t>
+  </si>
+  <si>
+    <t>Total Negatives</t>
+  </si>
+  <si>
+    <t>Total Observations</t>
+  </si>
+  <si>
+    <t>Roc Curve Data</t>
+  </si>
+  <si>
+    <t>Cutoff</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ActualPositives</t>
+  </si>
+  <si>
+    <t>ActualNegatives</t>
+  </si>
+  <si>
+    <t>PredictedPositives</t>
+  </si>
+  <si>
+    <t>PredictedNegatives</t>
+  </si>
+  <si>
+    <t>TruePositives</t>
+  </si>
+  <si>
+    <t>TrueNegatives</t>
+  </si>
+  <si>
+    <t>FalsePositives</t>
+  </si>
+  <si>
+    <t>FalseNegatives</t>
+  </si>
+  <si>
+    <t>Specificity</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>PositivePredictiveValue</t>
+  </si>
+  <si>
+    <t>NegativePredictiveValue</t>
+  </si>
+  <si>
+    <t>FalsePositiveRate</t>
+  </si>
+  <si>
+    <t>FalseDiscoveryRate</t>
+  </si>
+  <si>
+    <t>MatthewsCorrelationCoefficient</t>
+  </si>
+  <si>
+    <t>OddsRatio</t>
+  </si>
+  <si>
+    <t>Kappa</t>
+  </si>
+  <si>
+    <t>OverallDiagnosticPower</t>
+  </si>
+  <si>
+    <t>NormalizedMutualInformation</t>
+  </si>
+  <si>
+    <t>Random Roc</t>
+  </si>
+  <si>
+    <t>Roc Chart Ratio</t>
   </si>
 </sst>
 </file>
@@ -601,23 +716,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -637,6 +736,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -827,8 +942,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="197891200"/>
-        <c:axId val="197893120"/>
+        <c:axId val="224482432"/>
+        <c:axId val="224484352"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -953,11 +1068,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="199158400"/>
-        <c:axId val="199156864"/>
+        <c:axId val="224496256"/>
+        <c:axId val="224494720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="197891200"/>
+        <c:axId val="224482432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -981,12 +1096,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="197893120"/>
+        <c:crossAx val="224484352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="197893120"/>
+        <c:axId val="224484352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1021,12 +1136,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="197891200"/>
+        <c:crossAx val="224482432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="199156864"/>
+        <c:axId val="224494720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1062,14 +1177,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199158400"/>
+        <c:crossAx val="224496256"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
         <c:minorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="199158400"/>
+        <c:axId val="224496256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1079,7 +1194,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199156864"/>
+        <c:crossAx val="224494720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1095,9 +1210,322 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>ROC</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" baseline="0"/>
+              <a:t> Curve</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.9002974214264509E-2"/>
+          <c:y val="8.383488882655532E-2"/>
+          <c:w val="0.77094259655712027"/>
+          <c:h val="0.85716535181466702"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ROCData!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Roc Chart Ratio</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="28575">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>ROCData!$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:strRef>
+              <c:f>ROCData!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sensitivity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ROCData!$X$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ROCData!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random Roc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ROCData!$A$5:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ROCData!$B$5:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="267877760"/>
+        <c:axId val="267888128"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="267877760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.1000000000000001"/>
+          <c:min val="-0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr anchor="t" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>(1 - Specivity)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="267888128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="267888128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.1000000000000001"/>
+          <c:min val="-0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Sensitvity</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="267877760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
+  <sheetPr codeName="Chart2"/>
   <sheetViews>
     <sheetView zoomScale="131" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -1110,11 +1538,49 @@
 </chartsheet>
 </file>
 
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Chart4"/>
+  <sheetViews>
+    <sheetView zoomScale="135" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9255973" cy="6056737"/>
+    <xdr:ext cx="9285057" cy="6085821"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9299599" cy="6071279"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1145,6 +1611,38 @@
     <tableColumn id="2" name="Count"/>
     <tableColumn id="3" name="Percentage" dataDxfId="1"/>
     <tableColumn id="4" name="Cummlative %" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="RocTable" displayName="RocTable" ref="H1:AD1048576" totalsRowShown="0">
+  <autoFilter ref="H1:AD1048576"/>
+  <tableColumns count="23">
+    <tableColumn id="1" name="Cutoff"/>
+    <tableColumn id="2" name="Observations"/>
+    <tableColumn id="3" name="ActualPositives"/>
+    <tableColumn id="4" name="ActualNegatives"/>
+    <tableColumn id="5" name="PredictedPositives"/>
+    <tableColumn id="6" name="PredictedNegatives"/>
+    <tableColumn id="7" name="TruePositives"/>
+    <tableColumn id="8" name="TrueNegatives"/>
+    <tableColumn id="9" name="FalsePositives"/>
+    <tableColumn id="10" name="FalseNegatives"/>
+    <tableColumn id="11" name="Sensitivity"/>
+    <tableColumn id="12" name="Specificity"/>
+    <tableColumn id="13" name="Efficiency"/>
+    <tableColumn id="14" name="Accuracy"/>
+    <tableColumn id="15" name="PositivePredictiveValue"/>
+    <tableColumn id="16" name="NegativePredictiveValue"/>
+    <tableColumn id="17" name="FalsePositiveRate"/>
+    <tableColumn id="18" name="FalseDiscoveryRate"/>
+    <tableColumn id="19" name="MatthewsCorrelationCoefficient"/>
+    <tableColumn id="20" name="OddsRatio"/>
+    <tableColumn id="21" name="Kappa"/>
+    <tableColumn id="22" name="OverallDiagnosticPower"/>
+    <tableColumn id="23" name="NormalizedMutualInformation"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1437,10 +1935,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:G4"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,18 +1950,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
@@ -1471,46 +1970,46 @@
       <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+        <v>16</v>
+      </c>
+      <c r="B3" s="50"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="26">
         <v>123456789</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="25"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="48"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="53"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -1518,18 +2017,18 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="7"/>
       <c r="D5" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="25"/>
-      <c r="F5" s="44">
+      <c r="F5" s="54">
         <v>456123.4</v>
       </c>
-      <c r="G5" s="45"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
@@ -1538,21 +2037,21 @@
     <row r="6" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28"/>
       <c r="B6" s="28"/>
-      <c r="C6" s="46"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="28"/>
-      <c r="E6" s="46"/>
+      <c r="E6" s="40"/>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="41" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="32"/>
@@ -1582,37 +2081,37 @@
     </row>
     <row r="9" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
-      <c r="B9" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
+      <c r="B9" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
       <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:13" s="1" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="41" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="32"/>
@@ -1643,23 +2142,23 @@
     <row r="13" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
       <c r="B13" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
+        <v>32</v>
+      </c>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
       <c r="K13" s="24"/>
     </row>
     <row r="14" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -1684,29 +2183,35 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="H15" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="34"/>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
       <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="7">
+        <f>TestEndInstanceCount</f>
+        <v>50</v>
+      </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="37"/>
       <c r="C17" s="38">
@@ -1714,9 +2219,13 @@
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="G17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="7">
+        <f>C19</f>
+        <v>0</v>
+      </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
@@ -1729,9 +2238,13 @@
       <c r="C18" s="38"/>
       <c r="D18" s="25"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="G18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="7" t="b">
+        <f>TestEndInstanceCount=(H16+H17)</f>
+        <v>1</v>
+      </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
@@ -1753,13 +2266,13 @@
     </row>
     <row r="20" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="28"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
@@ -1769,17 +2282,17 @@
         <v>12</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>15</v>
@@ -1796,7 +2309,7 @@
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7">
-        <f>C22/TestEndInstanceCount</f>
+        <f>C22/Positives</f>
         <v>0</v>
       </c>
       <c r="E22" s="7"/>
@@ -1816,7 +2329,7 @@
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="e">
-        <f t="shared" ref="D23" si="0">C23/C18</f>
+        <f>C23/C18</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E23" s="7"/>
@@ -1951,7 +2464,7 @@
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -1961,6 +2474,114 @@
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1981,6 +2602,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2001,10 +2623,10 @@
         <v>15</v>
       </c>
       <c r="C1" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2188,6 +2810,178 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:AD8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="14.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="24.42578125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="25.28515625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="18.85546875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="20.28515625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="32" style="1" customWidth="1"/>
+    <col min="27" max="27" width="12.28515625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" style="1"/>
+    <col min="29" max="29" width="24.42578125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="30.42578125" style="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2202,7 +2996,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
@@ -2213,20 +3007,20 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="e">
         <f>MATCH(A2,C2:E2,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2234,8 +3028,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2249,7 +3044,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1">
         <v>1</v>

</xml_diff>